<commit_message>
Updated test script and added new test files Include a new gitignore file
</commit_message>
<xml_diff>
--- a/tests/valid-testdata/GIS_data.xlsx
+++ b/tests/valid-testdata/GIS_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://energinet-my.sharepoint.com/personal/tsp_energinet_dk/Documents/Dokumenter/Private Data/Projekter/DLR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9EA125EF-3A07-4503-858A-B66FEB0F9AC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{9EA125EF-3A07-4503-858A-B66FEB0F9AC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0673E95A-6D76-4A86-B6DB-DAA555B200C7}"/>
   <bookViews>
-    <workbookView xWindow="8760" yWindow="1485" windowWidth="26790" windowHeight="18390" xr2:uid="{E857CEF3-4D19-4743-8639-3B24CC5A23DB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{E857CEF3-4D19-4743-8639-3B24CC5A23DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -51,14 +51,14 @@
     <t>Lat_DD</t>
   </si>
   <si>
-    <t>EEE_150_FFF</t>
+    <t>EEE_150_FFF1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -76,6 +76,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -426,13 +432,13 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
@@ -523,6 +529,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>